<commit_message>
Added changes to the DCM piece of Motel 6
</commit_message>
<xml_diff>
--- a/DCM_CreativeDelivery_Motel6_DimensionList.xlsx
+++ b/DCM_CreativeDelivery_Motel6_DimensionList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4020"/>
   </bookViews>
   <sheets>
     <sheet name="Dimension" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>dfa:advertiser</t>
   </si>
   <si>
     <t>dfa:advertiserId</t>
-  </si>
-  <si>
-    <t>dfa:activeViewViewableImpressions</t>
   </si>
   <si>
     <t>dfa:richMediaBackupImages</t>
@@ -567,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,77 +585,77 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -668,7 +665,7 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -678,9 +675,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A33"/>
+  <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -694,12 +693,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -734,7 +733,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
@@ -744,7 +743,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -839,17 +838,12 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>